<commit_message>
Updated the frontend test database
</commit_message>
<xml_diff>
--- a/Feindesign/csv-mockup/frontend/frontend_test.xlsx
+++ b/Feindesign/csv-mockup/frontend/frontend_test.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hauss\Documents\Projektmanagement\yourChoice\Feindesign\csv-mockup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Projektmanagement\yourChoiceHO\Documentation\Feindesign\csv-mockup\frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053C45B1-52A9-47D4-A85F-E85A593C18CF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{34BDB0CF-8CF1-40A0-845B-65F3357F50D6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="voter" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
     <sheet name="client" sheetId="7" r:id="rId7"/>
     <sheet name="user" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="232">
   <si>
     <t>last_name</t>
   </si>
@@ -673,16 +672,67 @@
     <t>Wahl 1</t>
   </si>
   <si>
-    <t xml:space="preserve">2018-06-29T18:00:00.000Z </t>
-  </si>
-  <si>
     <t>2018-05-01T12:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2018-06-29T18:00:00.000Z</t>
+  </si>
+  <si>
+    <t>Bundestagswahl</t>
+  </si>
+  <si>
+    <t>Alternative für Deutschland</t>
+  </si>
+  <si>
+    <t>Christlich Demokratische Union Deutschlands</t>
+  </si>
+  <si>
+    <t>Sozialdemokratische Partei Deutschlands</t>
+  </si>
+  <si>
+    <t>Freie Demokratische Partei</t>
+  </si>
+  <si>
+    <t>AFD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>Gauland</t>
+  </si>
+  <si>
+    <t>Nahles</t>
+  </si>
+  <si>
+    <t>Andrea</t>
+  </si>
+  <si>
+    <t>Lindner</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Kramp-Karrenbauer</t>
+  </si>
+  <si>
+    <t>Annegret</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -717,7 +767,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1028,14 +1078,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD3FEF7-95AF-4D54-88B3-BBCC9717D633}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -1406,14 +1456,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C8784B-090B-4C40-81A9-BCD0613FD525}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
@@ -1446,16 +1496,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F73A539-73FB-4987-ACE5-0D13032795F0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
   </cols>
@@ -1485,22 +1536,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>0</v>
+      <c r="C2" t="s">
+        <v>215</v>
       </c>
       <c r="D2" t="s">
         <v>212</v>
       </c>
       <c r="E2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F2" t="s">
         <v>214</v>
-      </c>
-      <c r="F2" t="s">
-        <v>213</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -1512,14 +1563,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8FB308E-6B01-4A8F-8903-EC481A3B2332}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -1955,16 +2006,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C26A85-4717-458C-A606-8159023B6506}">
-  <dimension ref="A1:G21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -2455,20 +2506,112 @@
         <v>19</v>
       </c>
     </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>225</v>
+      </c>
+      <c r="B22" t="s">
+        <v>224</v>
+      </c>
+      <c r="C22" t="s">
+        <v>220</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>230</v>
+      </c>
+      <c r="B23" t="s">
+        <v>231</v>
+      </c>
+      <c r="C23" t="s">
+        <v>221</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>226</v>
+      </c>
+      <c r="B24" t="s">
+        <v>227</v>
+      </c>
+      <c r="C24" t="s">
+        <v>222</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>228</v>
+      </c>
+      <c r="B25" t="s">
+        <v>229</v>
+      </c>
+      <c r="C25" t="s">
+        <v>223</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40ECFD44-073D-46E6-9B17-FFE0E7200C63}">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="C22" sqref="C22:G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.85546875" bestFit="1" customWidth="1"/>
@@ -2476,7 +2619,7 @@
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>146</v>
       </c>
@@ -2495,8 +2638,11 @@
       <c r="F1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -2516,7 +2662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>149</v>
       </c>
@@ -2536,7 +2682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>151</v>
       </c>
@@ -2556,7 +2702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>178</v>
       </c>
@@ -2576,7 +2722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -2596,7 +2742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>179</v>
       </c>
@@ -2616,7 +2762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>157</v>
       </c>
@@ -2636,7 +2782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>180</v>
       </c>
@@ -2656,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>160</v>
       </c>
@@ -2676,7 +2822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>181</v>
       </c>
@@ -2696,7 +2842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>163</v>
       </c>
@@ -2716,7 +2862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>182</v>
       </c>
@@ -2736,7 +2882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>183</v>
       </c>
@@ -2756,7 +2902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>166</v>
       </c>
@@ -2776,7 +2922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>168</v>
       </c>
@@ -2796,7 +2942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>185</v>
       </c>
@@ -2816,7 +2962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>171</v>
       </c>
@@ -2836,7 +2982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>173</v>
       </c>
@@ -2856,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>186</v>
       </c>
@@ -2876,7 +3022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>176</v>
       </c>
@@ -2894,6 +3040,86 @@
       </c>
       <c r="F21">
         <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>216</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>50</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>217</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>51</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>218</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>52</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>219</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>53</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -2902,14 +3128,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565523F3-9A88-4699-83A1-1D991CC75B37}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2941,14 +3167,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC8CF70-D74C-4678-A518-7251564FE60E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Updated the database generation module. This simplifies the program call
</commit_message>
<xml_diff>
--- a/Feindesign/csv-mockup/frontend/frontend_test.xlsx
+++ b/Feindesign/csv-mockup/frontend/frontend_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="voter" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="235">
   <si>
     <t>last_name</t>
   </si>
@@ -727,6 +727,15 @@
   </si>
   <si>
     <t>Annegret</t>
+  </si>
+  <si>
+    <t>party_id</t>
+  </si>
+  <si>
+    <t>Europawahl</t>
+  </si>
+  <si>
+    <t>Wahl 2</t>
   </si>
 </sst>
 </file>
@@ -762,9 +771,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1081,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,10 +1507,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,6 +1565,29 @@
       </c>
       <c r="G2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E3" t="s">
+        <v>213</v>
+      </c>
+      <c r="F3" t="s">
+        <v>214</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2007,10 +2040,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2023,7 +2056,7 @@
     <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2045,8 +2078,11 @@
       <c r="G1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -2056,20 +2092,21 @@
       <c r="C2" t="s">
         <v>88</v>
       </c>
-      <c r="D2">
-        <v>55</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D2" s="2">
+        <v>55</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -2079,20 +2116,21 @@
       <c r="C3" t="s">
         <v>91</v>
       </c>
-      <c r="D3">
-        <v>55</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
+      <c r="D3" s="2">
+        <v>55</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -2102,20 +2140,21 @@
       <c r="C4" t="s">
         <v>94</v>
       </c>
-      <c r="D4">
-        <v>55</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
+      <c r="D4" s="2">
+        <v>55</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -2125,20 +2164,21 @@
       <c r="C5" t="s">
         <v>97</v>
       </c>
-      <c r="D5">
-        <v>55</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
+      <c r="D5" s="2">
+        <v>55</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -2148,20 +2188,21 @@
       <c r="C6" t="s">
         <v>100</v>
       </c>
-      <c r="D6">
-        <v>55</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
+      <c r="D6" s="2">
+        <v>55</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -2171,20 +2212,21 @@
       <c r="C7" t="s">
         <v>103</v>
       </c>
-      <c r="D7">
-        <v>55</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
+      <c r="D7" s="2">
+        <v>55</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -2194,20 +2236,21 @@
       <c r="C8" t="s">
         <v>106</v>
       </c>
-      <c r="D8">
-        <v>55</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
+      <c r="D8" s="2">
+        <v>55</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>107</v>
       </c>
@@ -2217,20 +2260,21 @@
       <c r="C9" t="s">
         <v>109</v>
       </c>
-      <c r="D9">
-        <v>55</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
+      <c r="D9" s="2">
+        <v>55</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>110</v>
       </c>
@@ -2240,20 +2284,21 @@
       <c r="C10" t="s">
         <v>112</v>
       </c>
-      <c r="D10">
-        <v>55</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
+      <c r="D10" s="2">
+        <v>55</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -2263,20 +2308,21 @@
       <c r="C11" t="s">
         <v>115</v>
       </c>
-      <c r="D11">
-        <v>55</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
+      <c r="D11" s="2">
+        <v>55</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>116</v>
       </c>
@@ -2286,20 +2332,21 @@
       <c r="C12" t="s">
         <v>118</v>
       </c>
-      <c r="D12">
-        <v>55</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
+      <c r="D12" s="2">
+        <v>55</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>119</v>
       </c>
@@ -2309,20 +2356,21 @@
       <c r="C13" t="s">
         <v>121</v>
       </c>
-      <c r="D13">
-        <v>55</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
+      <c r="D13" s="2">
+        <v>55</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>122</v>
       </c>
@@ -2332,20 +2380,21 @@
       <c r="C14" t="s">
         <v>124</v>
       </c>
-      <c r="D14">
-        <v>55</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
+      <c r="D14" s="2">
+        <v>55</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>125</v>
       </c>
@@ -2355,20 +2404,21 @@
       <c r="C15" t="s">
         <v>127</v>
       </c>
-      <c r="D15">
-        <v>55</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
+      <c r="D15" s="2">
+        <v>55</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -2378,20 +2428,21 @@
       <c r="C16" t="s">
         <v>130</v>
       </c>
-      <c r="D16">
-        <v>55</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
+      <c r="D16" s="2">
+        <v>55</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>131</v>
       </c>
@@ -2401,20 +2452,21 @@
       <c r="C17" t="s">
         <v>133</v>
       </c>
-      <c r="D17">
-        <v>55</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
+      <c r="D17" s="2">
+        <v>55</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>134</v>
       </c>
@@ -2424,20 +2476,21 @@
       <c r="C18" t="s">
         <v>136</v>
       </c>
-      <c r="D18">
-        <v>55</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
+      <c r="D18" s="2">
+        <v>55</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>137</v>
       </c>
@@ -2447,20 +2500,21 @@
       <c r="C19" t="s">
         <v>139</v>
       </c>
-      <c r="D19">
-        <v>55</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
+      <c r="D19" s="2">
+        <v>55</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>140</v>
       </c>
@@ -2470,20 +2524,21 @@
       <c r="C20" t="s">
         <v>142</v>
       </c>
-      <c r="D20">
-        <v>55</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
+      <c r="D20" s="2">
+        <v>55</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>143</v>
       </c>
@@ -2493,20 +2548,21 @@
       <c r="C21" t="s">
         <v>145</v>
       </c>
-      <c r="D21">
-        <v>55</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
+      <c r="D21" s="2">
+        <v>55</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>225</v>
       </c>
@@ -2516,20 +2572,23 @@
       <c r="C22" t="s">
         <v>220</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <v>2</v>
       </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
         <v>2</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>230</v>
       </c>
@@ -2539,20 +2598,23 @@
       <c r="C23" t="s">
         <v>221</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="2">
         <v>4</v>
       </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
         <v>2</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="2">
         <v>61</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>226</v>
       </c>
@@ -2562,20 +2624,23 @@
       <c r="C24" t="s">
         <v>222</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="2">
         <v>4</v>
       </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
         <v>2</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="2">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>228</v>
       </c>
@@ -2585,30 +2650,138 @@
       <c r="C25" t="s">
         <v>223</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
         <v>4</v>
       </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
         <v>2</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="2">
         <v>63</v>
+      </c>
+      <c r="H25" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>225</v>
+      </c>
+      <c r="B26" t="s">
+        <v>224</v>
+      </c>
+      <c r="C26" t="s">
+        <v>220</v>
+      </c>
+      <c r="D26" s="2">
+        <v>2</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>3</v>
+      </c>
+      <c r="G26" s="2">
+        <v>60</v>
+      </c>
+      <c r="H26" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>230</v>
+      </c>
+      <c r="B27" t="s">
+        <v>231</v>
+      </c>
+      <c r="C27" t="s">
+        <v>221</v>
+      </c>
+      <c r="D27" s="2">
+        <v>4</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>3</v>
+      </c>
+      <c r="G27" s="2">
+        <v>61</v>
+      </c>
+      <c r="H27" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>226</v>
+      </c>
+      <c r="B28" t="s">
+        <v>227</v>
+      </c>
+      <c r="C28" t="s">
+        <v>222</v>
+      </c>
+      <c r="D28" s="2">
+        <v>4</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>3</v>
+      </c>
+      <c r="G28" s="2">
+        <v>62</v>
+      </c>
+      <c r="H28" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>228</v>
+      </c>
+      <c r="B29" t="s">
+        <v>229</v>
+      </c>
+      <c r="C29" t="s">
+        <v>223</v>
+      </c>
+      <c r="D29" s="2">
+        <v>4</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>3</v>
+      </c>
+      <c r="G29" s="2">
+        <v>63</v>
+      </c>
+      <c r="H29" s="2">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:G25"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3119,6 +3292,86 @@
         <v>0</v>
       </c>
       <c r="G25" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>216</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>50</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>217</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>51</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>218</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>52</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>219</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>53</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
         <v>223</v>
       </c>
     </row>

</xml_diff>